<commit_message>
Journal de bord à jour
</commit_message>
<xml_diff>
--- a/Journaux de bord/Journal de bord Léo.xlsx
+++ b/Journaux de bord/Journal de bord Léo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -54,14 +54,64 @@
   </si>
   <si>
     <t>Fin du chapitre d'analyse</t>
+  </si>
+  <si>
+    <t>3h45min</t>
+  </si>
+  <si>
+    <t>1h30min</t>
+  </si>
+  <si>
+    <t>1h45min</t>
+  </si>
+  <si>
+    <t>Sqlite</t>
+  </si>
+  <si>
+    <t>Création de la base de données selon le MLD</t>
+  </si>
+  <si>
+    <t>Chapitre conception</t>
+  </si>
+  <si>
+    <t>Création d'un formulaire de Login</t>
+  </si>
+  <si>
+    <t>Fin du login + création de compte fonctionnel</t>
+  </si>
+  <si>
+    <t>Login fonctionnel + vue du frigo</t>
+  </si>
+  <si>
+    <t>Ajout d'un ingrédient (Design formulaire) + upload d'image fonctionnel</t>
+  </si>
+  <si>
+    <t>Ajout d'un ingrédient terminé</t>
+  </si>
+  <si>
+    <t>Modification d'un ingrédient</t>
+  </si>
+  <si>
+    <t>Modification d'un ingrédient terminé + événement clic sur une carte</t>
+  </si>
+  <si>
+    <t>Suppression d'un aliment terminé + message date de péremption</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -89,9 +139,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -385,16 +436,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -426,7 +477,148 @@
         <v>9</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>43445</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>43445</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>43445</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>43452</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>43473</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>43476</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>43480</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>43481</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>43483</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>43487</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>